<commit_message>
Fixes to incomplete parameter files.
</commit_message>
<xml_diff>
--- a/MendotaLake/ConfigurationInputsMendota.xlsx
+++ b/MendotaLake/ConfigurationInputsMendota.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ouyangzt/Documents/GLEON/SOS/MendotaLake/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16880" windowHeight="10980"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="16875" windowHeight="10980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>LakePerimeter</t>
   </si>
@@ -128,10 +123,16 @@
     <t>#Sediment</t>
   </si>
   <si>
-    <t>ObservedMAR</t>
-  </si>
-  <si>
     <t>g/m2/yr</t>
+  </si>
+  <si>
+    <t>ObservedMAR_oc</t>
+  </si>
+  <si>
+    <t>R_auto</t>
+  </si>
+  <si>
+    <t>POC_lc</t>
   </si>
 </sst>
 </file>
@@ -442,7 +443,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,15 +453,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -643,6 +644,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>0.8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
@@ -670,6 +682,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23">
+        <v>0.01</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
@@ -677,13 +700,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B25">
         <v>249</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>